<commit_message>
Add results of measurements
</commit_message>
<xml_diff>
--- a/Physics/3.4.2/3.4.2.xlsx
+++ b/Physics/3.4.2/3.4.2.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIPT-MIPS\Labs\Physics\3.4.2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6594FF76-CB94-4A40-90EE-5504B1F6C181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,31 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>\tau_0, мкс</t>
+  </si>
+  <si>
+    <t>\tau, мкс</t>
+  </si>
+  <si>
+    <t>T, С</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\sigma_T, C </t>
+  </si>
+  <si>
+    <t>\sigma_{\tau}, мкс</t>
+  </si>
+  <si>
+    <t>\delta_T, C</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -37,7 +66,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -45,15 +74,125 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +469,238 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="6" max="6" width="16.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8">
+        <v>6.9092000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B4" s="1">
+        <v>0.192</v>
+      </c>
+      <c r="C4" s="1">
+        <v>7.9379999999999997</v>
+      </c>
+      <c r="D4" s="2">
+        <v>14.19</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B5" s="3">
+        <v>0.192</v>
+      </c>
+      <c r="C5" s="3">
+        <v>7.9119999999999999</v>
+      </c>
+      <c r="D5" s="4">
+        <v>15.1</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B6" s="3">
+        <v>0.192</v>
+      </c>
+      <c r="C6" s="3">
+        <v>7.8769999999999998</v>
+      </c>
+      <c r="D6" s="4">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B7" s="3">
+        <v>0.192</v>
+      </c>
+      <c r="C7" s="3">
+        <v>7.8280000000000003</v>
+      </c>
+      <c r="D7" s="4">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B8" s="3">
+        <v>0.192</v>
+      </c>
+      <c r="C8" s="3">
+        <v>7.766</v>
+      </c>
+      <c r="D8" s="4">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B9" s="3">
+        <v>0.192</v>
+      </c>
+      <c r="C9" s="3">
+        <v>7.6859999999999999</v>
+      </c>
+      <c r="D9" s="4">
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B10" s="3">
+        <v>0.192</v>
+      </c>
+      <c r="C10" s="3">
+        <v>7.58</v>
+      </c>
+      <c r="D10" s="4">
+        <v>20.100000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B11" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C11" s="3">
+        <v>7.3760000000000003</v>
+      </c>
+      <c r="D11" s="4">
+        <v>22.08</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B12" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C12" s="3">
+        <v>7.2149999999999999</v>
+      </c>
+      <c r="D12" s="4">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B13" s="3">
+        <v>0.192</v>
+      </c>
+      <c r="C13" s="3">
+        <v>7.1429999999999998</v>
+      </c>
+      <c r="D13" s="4">
+        <v>26.08</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B14" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C14" s="3">
+        <v>7.1029999999999998</v>
+      </c>
+      <c r="D14" s="4">
+        <v>28.08</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B15" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C15" s="3">
+        <v>7.0780000000000003</v>
+      </c>
+      <c r="D15" s="4">
+        <v>30.09</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B16" s="3">
+        <v>0.37</v>
+      </c>
+      <c r="C16" s="3">
+        <v>7.0609999999999999</v>
+      </c>
+      <c r="D16" s="4">
+        <v>32.07</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="3">
+        <v>0.37</v>
+      </c>
+      <c r="C17" s="3">
+        <v>7.0469999999999997</v>
+      </c>
+      <c r="D17" s="4">
+        <v>34.08</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="3">
+        <v>0.37</v>
+      </c>
+      <c r="C18" s="3">
+        <v>7.0380000000000003</v>
+      </c>
+      <c r="D18" s="4">
+        <v>36.08</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="C19" s="3">
+        <v>7.0289999999999999</v>
+      </c>
+      <c r="D19" s="4">
+        <v>38.08</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B20" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="C20" s="5">
+        <v>7.0209999999999999</v>
+      </c>
+      <c r="D20" s="6">
+        <v>40.08</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 3.4.2 physics lab
</commit_message>
<xml_diff>
--- a/Physics/3.4.2/3.4.2.xlsx
+++ b/Physics/3.4.2/3.4.2.xlsx
@@ -8,17 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIPT-MIPS\Labs\Physics\3.4.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6594FF76-CB94-4A40-90EE-5504B1F6C181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38543658-F25E-4EF6-8119-FC092E49E934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -470,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:G20"/>
+  <dimension ref="B3:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="K4" sqref="K4:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,7 +491,7 @@
     <col min="6" max="6" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
@@ -499,7 +508,7 @@
         <v>6.9092000000000002</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4" s="1">
         <v>0.192</v>
       </c>
@@ -515,8 +524,16 @@
       <c r="G4" s="8">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I4">
+        <f>C4*C4-$G$3*$G$3</f>
+        <v>15.274799359999996</v>
+      </c>
+      <c r="K4">
+        <f>1/I4</f>
+        <v>6.5467308370589311E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
         <v>0.192</v>
       </c>
@@ -532,8 +549,16 @@
       <c r="G5" s="8">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I5">
+        <f t="shared" ref="I5:I20" si="0">C5*C5-$G$3*$G$3</f>
+        <v>14.862699360000001</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K20" si="1">1/I5</f>
+        <v>6.7282528952398862E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
         <v>0.192</v>
       </c>
@@ -544,8 +569,16 @@
         <v>16.100000000000001</v>
       </c>
       <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I6">
+        <f>C6*C6-$G$3*$G$3</f>
+        <v>14.310084359999998</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>6.9880789996964079E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7" s="3">
         <v>0.192</v>
       </c>
@@ -555,8 +588,16 @@
       <c r="D7" s="4">
         <v>17.100000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>13.540539360000004</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>7.385230184804098E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>0.192</v>
       </c>
@@ -566,8 +607,16 @@
       <c r="D8" s="4">
         <v>18.100000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>12.573711359999997</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>7.9531012870332041E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
         <v>0.192</v>
       </c>
@@ -577,8 +626,16 @@
       <c r="D9" s="4">
         <v>19.100000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>11.337551359999999</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>8.8202467027236484E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>0.192</v>
       </c>
@@ -588,8 +645,16 @@
       <c r="D10" s="4">
         <v>20.100000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>9.7193553600000016</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>0.10288748203563984</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>0.25</v>
       </c>
@@ -599,8 +664,16 @@
       <c r="D11" s="4">
         <v>22.08</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>6.6683313600000034</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>0.14996255375047821</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <v>0.25</v>
       </c>
@@ -610,8 +683,16 @@
       <c r="D12" s="4">
         <v>24.1</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>4.3191803599999972</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>0.23152540914035843</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <v>0.192</v>
       </c>
@@ -621,8 +702,16 @@
       <c r="D13" s="4">
         <v>26.08</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>3.285404359999994</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>0.3043765364699284</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <v>0.25</v>
       </c>
@@ -632,8 +721,16 @@
       <c r="D14" s="4">
         <v>28.08</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>2.7155643599999948</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>0.36824757856227053</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <v>0.25</v>
       </c>
@@ -643,8 +740,16 @@
       <c r="D15" s="4">
         <v>30.09</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>2.3610393600000066</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>0.42354228266656141</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <v>0.37</v>
       </c>
@@ -654,8 +759,16 @@
       <c r="D16" s="4">
         <v>32.07</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>2.1206763599999974</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>0.4715476717060218</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
         <v>0.37</v>
       </c>
@@ -665,8 +778,16 @@
       <c r="D17" s="4">
         <v>34.08</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>1.9231643599999941</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>0.51997635813093113</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B18" s="3">
         <v>0.37</v>
       </c>
@@ -676,8 +797,16 @@
       <c r="D18" s="4">
         <v>36.08</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>1.7963993600000023</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>0.55666909166567435</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B19" s="3">
         <v>0.4</v>
       </c>
@@ -687,8 +816,16 @@
       <c r="D19" s="4">
         <v>38.08</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>1.6697963599999994</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>0.59887542215027967</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B20" s="5">
         <v>0.4</v>
       </c>
@@ -697,6 +834,14 @@
       </c>
       <c r="D20" s="6">
         <v>40.08</v>
+      </c>
+      <c r="I20">
+        <f>C20*C20-$G$3*$G$3</f>
+        <v>1.5573963599999985</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>0.64209730142171451</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added last RC and Physics labs
</commit_message>
<xml_diff>
--- a/Physics/3.4.2/3.4.2.xlsx
+++ b/Physics/3.4.2/3.4.2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIPT-MIPS\Labs\Physics\3.4.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38543658-F25E-4EF6-8119-FC092E49E934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7955E40-8C67-4258-919B-60A7A09FC8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -482,7 +482,7 @@
   <dimension ref="B3:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K20"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -550,7 +550,7 @@
         <v>1E-3</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:I20" si="0">C5*C5-$G$3*$G$3</f>
+        <f t="shared" ref="I5:I19" si="0">C5*C5-$G$3*$G$3</f>
         <v>14.862699360000001</v>
       </c>
       <c r="K5">

</xml_diff>